<commit_message>
* Add topics page * Add conference venue page * Update featured sessions
</commit_message>
<xml_diff>
--- a/data/sessions.xlsx
+++ b/data/sessions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED319B-8508-4B06-950E-17A29732D18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB2ABE2-8DC1-4033-9D19-CDB7956E130A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>Dominic Magirr</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>Tobias Mütze</t>
+  </si>
+  <si>
+    <t>Statistics in Practice: Simulation studies as a tool to evaluate and compare the properties of statistical methods – an overview</t>
+  </si>
+  <si>
+    <t>Willi Sauerbrei</t>
   </si>
 </sst>
 </file>
@@ -701,12 +707,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1327,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2112F1F1-F72A-464A-B17D-4AAC4FF2BDB0}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -1364,16 +1373,24 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B4" xr:uid="{2112F1F1-F72A-464A-B17D-4AAC4FF2BDB0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B4">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B5">
       <sortCondition ref="A1:A4"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
* Update sessions * Add GMDS 2023
</commit_message>
<xml_diff>
--- a/data/sessions.xlsx
+++ b/data/sessions.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB2ABE2-8DC1-4033-9D19-CDB7956E130A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6125D4D0-D407-4593-9B18-648D2F172BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <sheet name="Featured Sessions" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Featured Sessions'!$A$1:$B$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Featured Sessions'!$A$1:$B$5</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Invited Sessions'!$A$1:$A$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Dominic Magirr</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>Willi Sauerbrei</t>
+  </si>
+  <si>
+    <t>Biometrical Journal Showcase - Editor’s Selection</t>
+  </si>
+  <si>
+    <t>Arne Bathke, Matthias Schmid</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1069,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1336,16 +1342,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2112F1F1-F72A-464A-B17D-4AAC4FF2BDB0}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="121.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1366,32 +1372,40 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B4" xr:uid="{2112F1F1-F72A-464A-B17D-4AAC4FF2BDB0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B5">
-      <sortCondition ref="A1:A4"/>
+  <autoFilter ref="A1:B5" xr:uid="{2112F1F1-F72A-464A-B17D-4AAC4FF2BDB0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B6">
+      <sortCondition ref="A1:A5"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* Update sessions * Add structure to homepage
</commit_message>
<xml_diff>
--- a/data/sessions.xlsx
+++ b/data/sessions.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6125D4D0-D407-4593-9B18-648D2F172BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC166E75-BE26-43EF-9853-92B8D1AD7FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invited Sessions" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Dominic Magirr</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Arne Bathke, Matthias Schmid</t>
+  </si>
+  <si>
+    <t>Arne Bathke, Johan Verbeeck</t>
   </si>
 </sst>
 </file>
@@ -1083,13 +1086,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="106.53515625" customWidth="1"/>
-    <col min="2" max="2" width="42.53515625" customWidth="1"/>
+    <col min="1" max="1" width="106.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1105,7 +1108,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -1121,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -1196,17 +1199,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA99BF6-BC4F-44D0-B55F-C4B4C344E7B9}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView zoomScale="155" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="155" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="121.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="121.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>44</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1238,7 +1241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
@@ -1246,7 +1249,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -1270,15 +1273,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1286,7 +1289,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>48</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>51</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1344,17 +1347,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2112F1F1-F72A-464A-B17D-4AAC4FF2BDB0}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="121.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="121.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -1362,7 +1365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1378,7 +1381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>57</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
* Add registration info * Add symposium and young stats session
</commit_message>
<xml_diff>
--- a/data/sessions.xlsx
+++ b/data/sessions.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC166E75-BE26-43EF-9853-92B8D1AD7FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B532D7FB-0A5D-4171-A968-70811703559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invited Sessions" sheetId="2" r:id="rId1"/>
     <sheet name="Topic-contributed Sessions" sheetId="3" r:id="rId2"/>
     <sheet name="Featured Sessions" sheetId="4" r:id="rId3"/>
+    <sheet name="Satellite Symposium" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Featured Sessions'!$A$1:$B$5</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>Dominic Magirr</t>
   </si>
@@ -207,6 +208,12 @@
   </si>
   <si>
     <t>Arne Bathke, Johan Verbeeck</t>
+  </si>
+  <si>
+    <t>Young Statisticians Sessions and Panel Discussion</t>
+  </si>
+  <si>
+    <t>Andrea Berghold, Stefanie Peschel</t>
   </si>
 </sst>
 </file>
@@ -716,9 +723,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1072,7 +1078,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1086,105 +1092,105 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="106.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="106.53515625" customWidth="1"/>
+    <col min="2" max="2" width="42.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1199,138 +1205,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA99BF6-BC4F-44D0-B55F-C4B4C344E7B9}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="155" workbookViewId="0">
+    <sheetView zoomScale="155" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="121.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="121.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B16" t="s">
@@ -1348,24 +1354,24 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A7" sqref="A7:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="121.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="121.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1381,7 +1387,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1389,20 +1395,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1414,4 +1420,43 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E2F733-27A6-41A8-8558-B4A53BCB372E}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="108.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.3828125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>